<commit_message>
delete comments and follow good practices is-archived extension id 56e87d9bdd462024aa41d66cc3f4306f67845c0c
</commit_message>
<xml_diff>
--- a/ig/nr/correctErrors/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/ig/nr/correctErrors/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-20T10:34:11+00:00</t>
+    <t>2023-03-20T10:37:48+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -647,7 +647,7 @@
     <t>isArchived</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/pdsm/StructureDefinition/PDSmIsArchived}
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/pdsm/StructureDefinition/pdsm-is-archived}
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
replace Expression with xpath 530e8e71f122bc0e38b954566ff7513da4f3dd91
</commit_message>
<xml_diff>
--- a/ig/nr/correctErrors/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/ig/nr/correctErrors/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-20T10:38:51+00:00</t>
+    <t>2023-03-20T10:43:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -411,7 +411,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-constr-cdr-maj:Elément requis lorsque le flux envoyé correspond à une mise à jour des données d’une fiche {null}</t>
+constr-cdr-maj:Elément requis lorsque le flux envoyé correspond à une mise à jour des données d’une fiche {f:meta/f:versionId}</t>
   </si>
   <si>
     <t>version : [0..1] Numerique</t>
@@ -838,7 +838,7 @@
  TRE_A04-TypeDocument-LOINC, OID : 2.16.840.1.113883.6.1
  TRE_A12-NomenclatureASTM, OID : ASTM
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J66-TypeCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J07-XdsTypeCode-CISIS peut être utilisé. {null}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J07-XdsTypeCode-CISIS peut être utilisé. {f:type}</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -896,7 +896,7 @@
 -	TRE_A03-ClasseDocument-CISIS, OID : 1.2.250.1.213.1.1.4.1
 -	TRE_A10-NomenclatureURN, OID : URN
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J57-ClassCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J06-XdsClassCode-CISIS peut être utilisé. {null}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J06-XdsClassCode-CISIS peut être utilisé. {f:category}</t>
   </si>
   <si>
     <t>Composition.class</t>
@@ -933,7 +933,7 @@
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 constr-subj-ref:La ressource référencée doit être présente sous l’élément DocumentReference.contained.
 Référence contrainte au profil FrPatient
-Cette même ressource est référencée depuis context.sourcePatientInfo. {null}</t>
+Cette même ressource est référencée depuis context.sourcePatientInfo. {f:subject}</t>
   </si>
   <si>
     <t>Event.subject</t>
@@ -1009,7 +1009,7 @@
 Reference contrainte à :
 - PractitionerRole : Dans le cas d’un auteur professionnel, c’est le profil PractitionerRoleOrganizationalRoleRASSreprésentant la situation d’exercice qui doit être référencé. Lui-même fera le lien avec le profil PractitionerRoleProfessionalRoleRASS représentant l’exercice professionnel et avec FrPractitioner.
 - Device,
-- Patient contrainte au profil FrPatient. {null}</t>
+- Patient contrainte au profil FrPatient. {f:author}</t>
   </si>
   <si>
     <t>Event.performer.actor</t>
@@ -1053,7 +1053,7 @@
 constr-bind-authenticator:Cardinalité contrainte à [1..1]
 Référence contrainte au profil 
 - PractitionerRole : Dans le cas d’un authentificateur professionnel, c’est le profil PractitionerRoleOrganizationalRoleRASS représentant la situation d’exercice qui doit être référencé. Lui-même fera le lien avec le profil PractitionerRoleProfessionalRoleRASS représentant l’exercice professionnel et avec FrPractitioner.
--  Organization contrainte au profil FrOrganization. {null}</t>
+-  Organization contrainte au profil FrOrganization. {f:authenticator}</t>
   </si>
   <si>
     <t>Composition.attester</t>
@@ -1119,7 +1119,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-constr-cdr-rempl:Elément requis lorsque le flux envoyé correspond au remplacement d'un document {null}constr-bind-relatesTo:Cardinalité contrainte à [1..1] lorsque le flux envoyé correspond au remplacement d’un document. {null}</t>
+constr-cdr-rempl:Elément requis lorsque le flux envoyé correspond au remplacement d'un document {f:relatesTo}constr-bind-relatesTo:Cardinalité contrainte à [1..1] lorsque le flux envoyé correspond au remplacement d’un document. {f:relatesTo}</t>
   </si>
   <si>
     <t>Composition.relatesTo</t>
@@ -1204,7 +1204,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-constr-bind-relatesToTarget:Référence contrainte au profil PDSm_ComprehensiveDocumentReference {null}</t>
+constr-bind-relatesToTarget:Référence contrainte au profil PDSm_ComprehensiveDocumentReference {f:relatesTo/f:target}</t>
   </si>
   <si>
     <t>Composition.relatesTo.target</t>
@@ -1266,7 +1266,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-constr-bind-securityLabel:Les codes pour cet élément doivent provenir du ValueSet spécifié par le standard. Lorsqu’aucun code ne correspond au concept recherché, un code provenant de la terminologie de référence TRE_A07-StatusVisibiliteDocument, OID : 1.2.250.1.213.1.1.4.13 peut être utilisé. {null}</t>
+constr-bind-securityLabel:Les codes pour cet élément doivent provenir du ValueSet spécifié par le standard. Lorsqu’aucun code ne correspond au concept recherché, un code provenant de la terminologie de référence TRE_A07-StatusVisibiliteDocument, OID : 1.2.250.1.213.1.1.4.13 peut être utilisé. {f:securityLabel}</t>
   </si>
   <si>
     <t>Composition.confidentiality, Composition.meta.security</t>
@@ -1459,7 +1459,7 @@
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 constr-bind-attachmenturl:Dans le cas de l’ajout de document, l’url fait référence à la ressource Binary (« Binary/[id] »).
-Dans le cas de la recherche, il s’agit de l’URL permettant d’accéder au document {null}</t>
+Dans le cas de la recherche, il s’agit de l’URL permettant d’accéder au document {f:content/f:attachment/f:url}</t>
   </si>
   <si>
     <t>./reference/literal</t>
@@ -1603,7 +1603,7 @@
 - TRE_A09-DICOMuidRegistry, OID : 1.2.840.10008.2.6.1
 - TRE_A10-NomenclatureURN, OID : URN
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J60-FormatCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J10-XdsFormatCode-CISIS peut être utilisé. {null}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J10-XdsFormatCode-CISIS peut être utilisé. {f:content/f:format}</t>
   </si>
   <si>
     <t>Composition.meta.profile</t>
@@ -1692,7 +1692,7 @@
 constr-bind-context-event:Nomenclatures utilisées :
 - CCAM pour les actes médicaux (OID="1.2.250.1.213.2.5");
 - CIM-10 pour les diagnostics de pathologie (OID="2.16.840.1.113883.6.3").
-- TRE_A00-ProducteurDocNonPS pour les documents d'expression personnelle du patient. {null}</t>
+- TRE_A00-ProducteurDocNonPS pour les documents d'expression personnelle du patient. {f:context/f:event}</t>
   </si>
   <si>
     <t>Composition.event.code</t>
@@ -1823,7 +1823,7 @@
 -	TRE_A00-ProducteurDocNonPS, OID : 1.2.250.1.213.1.1.4.6 (lorsque l’auteur du document est un patient ou un équipement sous sa responsabilité)
 -	TRE_R02-SecteurActivite, OID : 1.2.250.1.71.4.2.4 (lorsque l’auteur du document est un professionnel ou un équipement sous sa responsabilité)
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J61-HealthcareFacilityTypeCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J02-XdsHealthcareFacilityTypeCode-CISIS peut être utilisé. {null}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J02-XdsHealthcareFacilityTypeCode-CISIS peut être utilisé. {f:context/f:facilityType or f:context/f:practiceSetting}</t>
   </si>
   <si>
     <t>usually from a mapping to a local ValueSet</t>

</xml_diff>